<commit_message>
Contabilidad 1 continuar en casa
Conta 1 continuar en casa
</commit_message>
<xml_diff>
--- a/Coursera/05-Contabilidad_Financiera/ejercicio1.xlsx
+++ b/Coursera/05-Contabilidad_Financiera/ejercicio1.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmedina\Downloads\Curso Angular\Angular\Coursera\05-Contabilidad_Financiera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77153B4C-799B-4901-AC7A-F98004F3F398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C410CBF4-92B6-4D7D-A6E4-63E3565FDAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20490" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{B931288A-4DE7-46F8-86FA-F5D655DBF73D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{B931288A-4DE7-46F8-86FA-F5D655DBF73D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Ejercicios de Contabilidad</t>
   </si>
@@ -73,12 +72,36 @@
   </si>
   <si>
     <t>alquiler adelantado</t>
+  </si>
+  <si>
+    <t>1 Capital aportado</t>
+  </si>
+  <si>
+    <t>Aplicaiones del capital</t>
+  </si>
+  <si>
+    <t>Origigenes del Capital</t>
+  </si>
+  <si>
+    <t>Capital Social</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Prestamos Bancarios</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-C0A]_-;\-* #,##0.00\ [$€-C0A]_-;_-* &quot;-&quot;??\ [$€-C0A]_-;_-@_-"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,16 +154,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,8 +192,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1323975</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>80484</xdr:rowOff>
     </xdr:to>
@@ -524,133 +548,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB6C87B-A04E-4DF6-85F2-4008AA5B039E}">
-  <dimension ref="B1:I27"/>
+  <dimension ref="B1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="2" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="5">
+        <v>50000</v>
+      </c>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="2" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="3" t="s">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="5">
+        <v>50000</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="4" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="5">
+        <v>20000</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <v>50000</v>
       </c>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="4" t="s">
+      <c r="F19" s="2"/>
+      <c r="I19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <v>20000</v>
       </c>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="4" t="s">
+      <c r="F20" s="2"/>
+      <c r="I20" s="5"/>
+      <c r="J20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="5">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <f>+E19+E20</f>
         <v>70000</v>
       </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="3" t="s">
+      <c r="F21" s="2"/>
+      <c r="I21" s="5"/>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="5">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="4" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="I23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <v>15000</v>
       </c>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="4" t="s">
+      <c r="F24" s="2"/>
+      <c r="I24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2">
         <v>3000</v>
       </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="4" t="s">
+      <c r="I25" s="5"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2">
         <v>6000</v>
       </c>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D27" s="4" t="s">
+      <c r="I26" s="5"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="2">
         <f>+F26+F25+E24</f>
         <v>24000</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="2"/>
+      <c r="I27" s="5"/>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I28" s="5"/>
+      <c r="K28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>